<commit_message>
updated wording on profiles, added google scholar links to profiles (icon and hyperlink). Re-oredered gallery
</commit_message>
<xml_diff>
--- a/website_content_creation/Author_form.xlsx
+++ b/website_content_creation/Author_form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>** administrative category, for after receipt.</t>
+  </si>
+  <si>
+    <t>Google Scholar</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -517,24 +520,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1001"/>
+  <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B34"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -814,113 +818,115 @@
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="24"/>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-    </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+    </row>
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C16" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-    </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="25"/>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="38"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="28"/>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="30"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="26"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="30"/>
-    </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="29"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="28"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="28"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="27"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
@@ -930,28 +936,31 @@
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-    </row>
     <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-    </row>
-    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
+      <c r="A34" s="20"/>
+    </row>
+    <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
     </row>
     <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29"/>
+      <c r="A36" s="33"/>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-    </row>
-    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A37" s="27"/>
+    </row>
+    <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+    </row>
     <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1915,10 +1924,11 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
updated author profiles & author page creation script, author details form to include OrcIDs. Updated Instagram with more recent posts.
</commit_message>
<xml_diff>
--- a/website_content_creation/Author_form.xlsx
+++ b/website_content_creation/Author_form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Google Scholar</t>
+  </si>
+  <si>
+    <t>OrcID</t>
   </si>
 </sst>
 </file>
@@ -529,6 +532,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,7 +542,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1002"/>
+  <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -818,119 +821,121 @@
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="34" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-    </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="29" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B17" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C17" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-    </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="38"/>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="B24" s="39"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="26"/>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="28"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="26"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="28"/>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="27"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="28"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="B29" s="27"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
@@ -940,28 +945,31 @@
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+    </row>
+    <row r="33" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-    </row>
     <row r="35" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-    </row>
-    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="33"/>
+      <c r="A35" s="20"/>
+    </row>
+    <row r="36" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
     </row>
     <row r="37" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
+      <c r="A37" s="33"/>
     </row>
     <row r="38" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-    </row>
-    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A38" s="27"/>
+    </row>
+    <row r="39" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+    </row>
     <row r="40" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1925,10 +1933,11 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Updated Instagram feed, updated E.Emilson profile, added grad student posting, republished
</commit_message>
<xml_diff>
--- a/website_content_creation/Author_form.xlsx
+++ b/website_content_creation/Author_form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Website Profile Form</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>OrcID</t>
+  </si>
+  <si>
+    <t>** Fill out a little personal bio blurb</t>
+  </si>
+  <si>
+    <t>** any other information you would like on your profile.</t>
   </si>
 </sst>
 </file>
@@ -760,7 +766,7 @@
   <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -843,12 +849,18 @@
         <v>19</v>
       </c>
       <c r="B12" s="24"/>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="5"/>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">

</xml_diff>

<commit_message>
Removed Twitter and added instagram links
</commit_message>
<xml_diff>
--- a/website_content_creation/Author_form.xlsx
+++ b/website_content_creation/Author_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{4AA7E540-252E-417C-AC05-0559222007F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9095C315-D83F-4DCD-BBF4-FBF8C307480A}"/>
   <bookViews>
-    <workbookView xWindow="-14235" yWindow="-16395" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12765" yWindow="-15045" windowWidth="27000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>Twitter</t>
-  </si>
-  <si>
     <t>e-mail</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>** Canada government profile page</t>
+  </si>
+  <si>
+    <t>Instagram</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:C1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -803,107 +803,107 @@
       </c>
       <c r="B4" s="20"/>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
+      <c r="A5" s="31" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="C18" s="28" t="s">
         <v>13</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,16 +934,16 @@
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="36"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>